<commit_message>
Added a readObservedData function to incapsulate calls to ospsuite::loadDataSetsFromExcel
</commit_message>
<xml_diff>
--- a/tests/dev/Data/DataSet.xlsx
+++ b/tests/dev/Data/DataSet.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite.ParameterIdentification\tests\dev\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svavil\Downloads\esqlabs\OSPSuite.ParameterIdentification\tests\dev\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F493C-4F71-43CB-A40F-8A4A4A16F484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1B4625-C6ED-4C6F-A1BF-E5B994930148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="28800" windowHeight="18940" tabRatio="875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boswell_2012" sheetId="64" r:id="rId1"/>
-    <sheet name="Boswell_2012_Error" sheetId="65" r:id="rId2"/>
-    <sheet name="MetaInfo" sheetId="48" r:id="rId3"/>
+    <sheet name="MetaInfo" sheetId="48" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>Study Id</t>
   </si>
@@ -59,9 +58,6 @@
   </si>
   <si>
     <t>Route</t>
-  </si>
-  <si>
-    <t>Group Id</t>
   </si>
   <si>
     <t>Backer_1989</t>
@@ -180,6 +176,9 @@
   </si>
   <si>
     <t>MW</t>
+  </si>
+  <si>
+    <t>PK</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FB60DA-1FD0-45A2-84E9-D44628671A39}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:N51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,22 +1097,22 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
         <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1121,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>176.85118</v>
+        <v>173.25665000000001</v>
       </c>
       <c r="N2" t="s">
         <v>19</v>
@@ -1132,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="K3">
-        <v>219.98562999999999</v>
+        <v>251.61753999999999</v>
       </c>
       <c r="N3" t="s">
         <v>19</v>
@@ -1143,7 +1142,7 @@
         <v>8</v>
       </c>
       <c r="K4">
-        <v>263.12006000000002</v>
+        <v>224.29907</v>
       </c>
       <c r="N4" t="s">
         <v>19</v>
@@ -1154,7 +1153,7 @@
         <v>11</v>
       </c>
       <c r="K5">
-        <v>331.41626000000002</v>
+        <v>282.53055000000001</v>
       </c>
       <c r="N5" t="s">
         <v>19</v>
@@ -1165,7 +1164,7 @@
         <v>15</v>
       </c>
       <c r="K6">
-        <v>385.33429999999998</v>
+        <v>334.29187000000002</v>
       </c>
       <c r="N6" t="s">
         <v>19</v>
@@ -1176,7 +1175,7 @@
         <v>19</v>
       </c>
       <c r="K7">
-        <v>431.34435999999999</v>
+        <v>360.17255</v>
       </c>
       <c r="N7" t="s">
         <v>19</v>
@@ -1187,7 +1186,7 @@
         <v>22</v>
       </c>
       <c r="K8">
-        <v>524.08339999999998</v>
+        <v>405.46368000000001</v>
       </c>
       <c r="N8" t="s">
         <v>19</v>
@@ -1198,7 +1197,7 @@
         <v>25</v>
       </c>
       <c r="K9">
-        <v>561.46654999999998</v>
+        <v>512.58090000000004</v>
       </c>
       <c r="N9" t="s">
         <v>19</v>
@@ -1209,7 +1208,7 @@
         <v>30</v>
       </c>
       <c r="K10">
-        <v>647.01653999999996</v>
+        <v>588.78503000000001</v>
       </c>
       <c r="N10" t="s">
         <v>19</v>
@@ -1220,7 +1219,7 @@
         <v>33</v>
       </c>
       <c r="K11">
-        <v>706.68584999999996</v>
+        <v>693.02660000000003</v>
       </c>
       <c r="N11" t="s">
         <v>19</v>
@@ -1231,7 +1230,7 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <v>173.25665000000001</v>
+        <v>168.94319999999999</v>
       </c>
       <c r="N12" t="s">
         <v>20</v>
@@ -1242,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="K13">
-        <v>251.61753999999999</v>
+        <v>214.95328000000001</v>
       </c>
       <c r="N13" t="s">
         <v>20</v>
@@ -1264,7 +1263,7 @@
         <v>11</v>
       </c>
       <c r="K15">
-        <v>282.53055000000001</v>
+        <v>269.59019999999998</v>
       </c>
       <c r="N15" t="s">
         <v>20</v>
@@ -1275,7 +1274,7 @@
         <v>15</v>
       </c>
       <c r="K16">
-        <v>334.29187000000002</v>
+        <v>306.97340000000003</v>
       </c>
       <c r="N16" t="s">
         <v>20</v>
@@ -1286,7 +1285,7 @@
         <v>19</v>
       </c>
       <c r="K17">
-        <v>360.17255</v>
+        <v>352.98345999999998</v>
       </c>
       <c r="N17" t="s">
         <v>20</v>
@@ -1297,7 +1296,7 @@
         <v>22</v>
       </c>
       <c r="K18">
-        <v>405.46368000000001</v>
+        <v>407.62042000000002</v>
       </c>
       <c r="N18" t="s">
         <v>20</v>
@@ -1308,7 +1307,7 @@
         <v>25</v>
       </c>
       <c r="K19">
-        <v>512.58090000000004</v>
+        <v>483.82459999999998</v>
       </c>
       <c r="N19" t="s">
         <v>20</v>
@@ -1319,7 +1318,7 @@
         <v>30</v>
       </c>
       <c r="K20">
-        <v>588.78503000000001</v>
+        <v>610.35230000000001</v>
       </c>
       <c r="N20" t="s">
         <v>20</v>
@@ -1330,7 +1329,7 @@
         <v>33</v>
       </c>
       <c r="K21">
-        <v>693.02660000000003</v>
+        <v>683.68079999999998</v>
       </c>
       <c r="N21" t="s">
         <v>20</v>
@@ -1341,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="K22">
-        <v>168.94319999999999</v>
+        <v>173.25665000000001</v>
       </c>
       <c r="N22" t="s">
         <v>21</v>
@@ -1352,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="K23">
-        <v>214.95328000000001</v>
+        <v>231.48813999999999</v>
       </c>
       <c r="N23" t="s">
         <v>21</v>
@@ -1363,7 +1362,7 @@
         <v>8</v>
       </c>
       <c r="K24">
-        <v>224.29907</v>
+        <v>178.28899999999999</v>
       </c>
       <c r="N24" t="s">
         <v>21</v>
@@ -1374,7 +1373,7 @@
         <v>11</v>
       </c>
       <c r="K25">
-        <v>269.59019999999998</v>
+        <v>242.27173999999999</v>
       </c>
       <c r="N25" t="s">
         <v>21</v>
@@ -1385,7 +1384,7 @@
         <v>15</v>
       </c>
       <c r="K26">
-        <v>306.97340000000003</v>
+        <v>264.55786000000001</v>
       </c>
       <c r="N26" t="s">
         <v>21</v>
@@ -1396,7 +1395,7 @@
         <v>19</v>
       </c>
       <c r="K27">
-        <v>352.98345999999998</v>
+        <v>268.1524</v>
       </c>
       <c r="N27" t="s">
         <v>21</v>
@@ -1407,7 +1406,7 @@
         <v>22</v>
       </c>
       <c r="K28">
-        <v>407.62042000000002</v>
+        <v>291.87634000000003</v>
       </c>
       <c r="N28" t="s">
         <v>21</v>
@@ -1418,7 +1417,7 @@
         <v>25</v>
       </c>
       <c r="K29">
-        <v>483.82459999999998</v>
+        <v>322.07047</v>
       </c>
       <c r="N29" t="s">
         <v>21</v>
@@ -1429,7 +1428,7 @@
         <v>30</v>
       </c>
       <c r="K30">
-        <v>610.35230000000001</v>
+        <v>443.56576999999999</v>
       </c>
       <c r="N30" t="s">
         <v>21</v>
@@ -1440,7 +1439,7 @@
         <v>33</v>
       </c>
       <c r="K31">
-        <v>683.68079999999998</v>
+        <v>516.89435000000003</v>
       </c>
       <c r="N31" t="s">
         <v>21</v>
@@ -1451,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="K32">
-        <v>173.25665000000001</v>
+        <v>176.85118</v>
       </c>
       <c r="N32" t="s">
         <v>22</v>
@@ -1462,7 +1461,7 @@
         <v>4</v>
       </c>
       <c r="K33">
-        <v>231.48813999999999</v>
+        <v>226.45578</v>
       </c>
       <c r="N33" t="s">
         <v>22</v>
@@ -1473,7 +1472,7 @@
         <v>8</v>
       </c>
       <c r="K34">
-        <v>178.28899999999999</v>
+        <v>217.8289</v>
       </c>
       <c r="N34" t="s">
         <v>22</v>
@@ -1484,7 +1483,7 @@
         <v>11</v>
       </c>
       <c r="K35">
-        <v>242.27173999999999</v>
+        <v>294.75198</v>
       </c>
       <c r="N35" t="s">
         <v>22</v>
@@ -1495,7 +1494,7 @@
         <v>15</v>
       </c>
       <c r="K36">
-        <v>264.55786000000001</v>
+        <v>299.06542999999999</v>
       </c>
       <c r="N36" t="s">
         <v>22</v>
@@ -1506,7 +1505,7 @@
         <v>19</v>
       </c>
       <c r="K37">
-        <v>268.1524</v>
+        <v>308.41122000000001</v>
       </c>
       <c r="N37" t="s">
         <v>22</v>
@@ -1517,7 +1516,7 @@
         <v>22</v>
       </c>
       <c r="K38">
-        <v>291.87634000000003</v>
+        <v>331.41626000000002</v>
       </c>
       <c r="N38" t="s">
         <v>22</v>
@@ -1528,7 +1527,7 @@
         <v>25</v>
       </c>
       <c r="K39">
-        <v>322.07047</v>
+        <v>390.36664000000002</v>
       </c>
       <c r="N39" t="s">
         <v>22</v>
@@ -1539,7 +1538,7 @@
         <v>30</v>
       </c>
       <c r="K40">
-        <v>443.56576999999999</v>
+        <v>462.97629999999998</v>
       </c>
       <c r="N40" t="s">
         <v>22</v>
@@ -1550,7 +1549,7 @@
         <v>33</v>
       </c>
       <c r="K41">
-        <v>516.89435000000003</v>
+        <v>539.89935000000003</v>
       </c>
       <c r="N41" t="s">
         <v>22</v>
@@ -1564,7 +1563,7 @@
         <v>176.85118</v>
       </c>
       <c r="N42" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="10:14" x14ac:dyDescent="0.35">
@@ -1572,10 +1571,10 @@
         <v>4</v>
       </c>
       <c r="K43">
-        <v>226.45578</v>
+        <v>219.98562999999999</v>
       </c>
       <c r="N43" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="10:14" x14ac:dyDescent="0.35">
@@ -1583,10 +1582,10 @@
         <v>8</v>
       </c>
       <c r="K44">
-        <v>217.8289</v>
+        <v>263.12006000000002</v>
       </c>
       <c r="N44" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="10:14" x14ac:dyDescent="0.35">
@@ -1594,10 +1593,10 @@
         <v>11</v>
       </c>
       <c r="K45">
-        <v>294.75198</v>
+        <v>331.41626000000002</v>
       </c>
       <c r="N45" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="10:14" x14ac:dyDescent="0.35">
@@ -1605,10 +1604,10 @@
         <v>15</v>
       </c>
       <c r="K46">
-        <v>299.06542999999999</v>
+        <v>385.33429999999998</v>
       </c>
       <c r="N46" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="10:14" x14ac:dyDescent="0.35">
@@ -1616,10 +1615,10 @@
         <v>19</v>
       </c>
       <c r="K47">
-        <v>308.41122000000001</v>
+        <v>431.34435999999999</v>
       </c>
       <c r="N47" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="10:14" x14ac:dyDescent="0.35">
@@ -1627,10 +1626,10 @@
         <v>22</v>
       </c>
       <c r="K48">
-        <v>331.41626000000002</v>
+        <v>524.08339999999998</v>
       </c>
       <c r="N48" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="10:14" x14ac:dyDescent="0.35">
@@ -1638,10 +1637,10 @@
         <v>25</v>
       </c>
       <c r="K49">
-        <v>390.36664000000002</v>
+        <v>561.46654999999998</v>
       </c>
       <c r="N49" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="10:14" x14ac:dyDescent="0.35">
@@ -1649,10 +1648,10 @@
         <v>30</v>
       </c>
       <c r="K50">
-        <v>462.97629999999998</v>
+        <v>647.01653999999996</v>
       </c>
       <c r="N50" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="10:14" x14ac:dyDescent="0.35">
@@ -1660,827 +1659,22 @@
         <v>33</v>
       </c>
       <c r="K51">
-        <v>539.89935000000003</v>
+        <v>706.68584999999996</v>
       </c>
       <c r="N51" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N51">
+    <sortCondition ref="N2:N51"/>
+    <sortCondition ref="J2:J51"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E130360-29C4-4F79-90A7-EBE9DBEF9F87}">
-  <dimension ref="A24:N74"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25:L74"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K24" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>176.85118</v>
-      </c>
-      <c r="L25">
-        <f>K25*0.1</f>
-        <v>17.685117999999999</v>
-      </c>
-      <c r="N25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J26">
-        <v>4</v>
-      </c>
-      <c r="K26">
-        <v>219.98562999999999</v>
-      </c>
-      <c r="L26">
-        <f t="shared" ref="L26:L74" si="0">K26*0.1</f>
-        <v>21.998563000000001</v>
-      </c>
-      <c r="N26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J27">
-        <v>8</v>
-      </c>
-      <c r="K27">
-        <v>263.12006000000002</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
-        <v>26.312006000000004</v>
-      </c>
-      <c r="N27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J28">
-        <v>11</v>
-      </c>
-      <c r="K28">
-        <v>331.41626000000002</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
-        <v>33.141626000000002</v>
-      </c>
-      <c r="N28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J29">
-        <v>15</v>
-      </c>
-      <c r="K29">
-        <v>385.33429999999998</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="0"/>
-        <v>38.533430000000003</v>
-      </c>
-      <c r="N29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J30">
-        <v>19</v>
-      </c>
-      <c r="K30">
-        <v>431.34435999999999</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="0"/>
-        <v>43.134436000000001</v>
-      </c>
-      <c r="N30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J31">
-        <v>22</v>
-      </c>
-      <c r="K31">
-        <v>524.08339999999998</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
-        <v>52.408340000000003</v>
-      </c>
-      <c r="N31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J32">
-        <v>25</v>
-      </c>
-      <c r="K32">
-        <v>561.46654999999998</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="0"/>
-        <v>56.146655000000003</v>
-      </c>
-      <c r="N32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J33">
-        <v>30</v>
-      </c>
-      <c r="K33">
-        <v>647.01653999999996</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="0"/>
-        <v>64.701654000000005</v>
-      </c>
-      <c r="N33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J34">
-        <v>33</v>
-      </c>
-      <c r="K34">
-        <v>706.68584999999996</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="0"/>
-        <v>70.668584999999993</v>
-      </c>
-      <c r="N34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="K35">
-        <v>173.25665000000001</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="0"/>
-        <v>17.325665000000001</v>
-      </c>
-      <c r="N35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J36">
-        <v>4</v>
-      </c>
-      <c r="K36">
-        <v>251.61753999999999</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="0"/>
-        <v>25.161754000000002</v>
-      </c>
-      <c r="N36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J37">
-        <v>8</v>
-      </c>
-      <c r="K37">
-        <v>224.29907</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="0"/>
-        <v>22.429907</v>
-      </c>
-      <c r="N37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J38">
-        <v>11</v>
-      </c>
-      <c r="K38">
-        <v>282.53055000000001</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="0"/>
-        <v>28.253055000000003</v>
-      </c>
-      <c r="N38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J39">
-        <v>15</v>
-      </c>
-      <c r="K39">
-        <v>334.29187000000002</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="0"/>
-        <v>33.429187000000006</v>
-      </c>
-      <c r="N39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J40">
-        <v>19</v>
-      </c>
-      <c r="K40">
-        <v>360.17255</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="0"/>
-        <v>36.017254999999999</v>
-      </c>
-      <c r="N40" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J41">
-        <v>22</v>
-      </c>
-      <c r="K41">
-        <v>405.46368000000001</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="0"/>
-        <v>40.546368000000001</v>
-      </c>
-      <c r="N41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J42">
-        <v>25</v>
-      </c>
-      <c r="K42">
-        <v>512.58090000000004</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="0"/>
-        <v>51.25809000000001</v>
-      </c>
-      <c r="N42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J43">
-        <v>30</v>
-      </c>
-      <c r="K43">
-        <v>588.78503000000001</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="0"/>
-        <v>58.878503000000002</v>
-      </c>
-      <c r="N43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J44">
-        <v>33</v>
-      </c>
-      <c r="K44">
-        <v>693.02660000000003</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="0"/>
-        <v>69.302660000000003</v>
-      </c>
-      <c r="N44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J45">
-        <v>1</v>
-      </c>
-      <c r="K45">
-        <v>168.94319999999999</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="0"/>
-        <v>16.89432</v>
-      </c>
-      <c r="N45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J46">
-        <v>4</v>
-      </c>
-      <c r="K46">
-        <v>214.95328000000001</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="0"/>
-        <v>21.495328000000001</v>
-      </c>
-      <c r="N46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J47">
-        <v>8</v>
-      </c>
-      <c r="K47">
-        <v>224.29907</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="0"/>
-        <v>22.429907</v>
-      </c>
-      <c r="N47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J48">
-        <v>11</v>
-      </c>
-      <c r="K48">
-        <v>269.59019999999998</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="0"/>
-        <v>26.959019999999999</v>
-      </c>
-      <c r="N48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J49">
-        <v>15</v>
-      </c>
-      <c r="K49">
-        <v>306.97340000000003</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="0"/>
-        <v>30.697340000000004</v>
-      </c>
-      <c r="N49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J50">
-        <v>19</v>
-      </c>
-      <c r="K50">
-        <v>352.98345999999998</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="0"/>
-        <v>35.298346000000002</v>
-      </c>
-      <c r="N50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J51">
-        <v>22</v>
-      </c>
-      <c r="K51">
-        <v>407.62042000000002</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="0"/>
-        <v>40.762042000000008</v>
-      </c>
-      <c r="N51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J52">
-        <v>25</v>
-      </c>
-      <c r="K52">
-        <v>483.82459999999998</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
-        <v>48.382460000000002</v>
-      </c>
-      <c r="N52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J53">
-        <v>30</v>
-      </c>
-      <c r="K53">
-        <v>610.35230000000001</v>
-      </c>
-      <c r="L53">
-        <f t="shared" si="0"/>
-        <v>61.035230000000006</v>
-      </c>
-      <c r="N53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J54">
-        <v>33</v>
-      </c>
-      <c r="K54">
-        <v>683.68079999999998</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="0"/>
-        <v>68.368080000000006</v>
-      </c>
-      <c r="N54" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J55">
-        <v>1</v>
-      </c>
-      <c r="K55">
-        <v>173.25665000000001</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="0"/>
-        <v>17.325665000000001</v>
-      </c>
-      <c r="N55" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J56">
-        <v>4</v>
-      </c>
-      <c r="K56">
-        <v>231.48813999999999</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="0"/>
-        <v>23.148814000000002</v>
-      </c>
-      <c r="N56" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J57">
-        <v>8</v>
-      </c>
-      <c r="K57">
-        <v>178.28899999999999</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
-        <v>17.828900000000001</v>
-      </c>
-      <c r="N57" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J58">
-        <v>11</v>
-      </c>
-      <c r="K58">
-        <v>242.27173999999999</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="0"/>
-        <v>24.227174000000002</v>
-      </c>
-      <c r="N58" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J59">
-        <v>15</v>
-      </c>
-      <c r="K59">
-        <v>264.55786000000001</v>
-      </c>
-      <c r="L59">
-        <f t="shared" si="0"/>
-        <v>26.455786000000003</v>
-      </c>
-      <c r="N59" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J60">
-        <v>19</v>
-      </c>
-      <c r="K60">
-        <v>268.1524</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="0"/>
-        <v>26.815240000000003</v>
-      </c>
-      <c r="N60" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J61">
-        <v>22</v>
-      </c>
-      <c r="K61">
-        <v>291.87634000000003</v>
-      </c>
-      <c r="L61">
-        <f t="shared" si="0"/>
-        <v>29.187634000000003</v>
-      </c>
-      <c r="N61" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J62">
-        <v>25</v>
-      </c>
-      <c r="K62">
-        <v>322.07047</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="0"/>
-        <v>32.207047000000003</v>
-      </c>
-      <c r="N62" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J63">
-        <v>30</v>
-      </c>
-      <c r="K63">
-        <v>443.56576999999999</v>
-      </c>
-      <c r="L63">
-        <f t="shared" si="0"/>
-        <v>44.356577000000001</v>
-      </c>
-      <c r="N63" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J64">
-        <v>33</v>
-      </c>
-      <c r="K64">
-        <v>516.89435000000003</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="0"/>
-        <v>51.689435000000003</v>
-      </c>
-      <c r="N64" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J65">
-        <v>1</v>
-      </c>
-      <c r="K65">
-        <v>176.85118</v>
-      </c>
-      <c r="L65">
-        <f t="shared" si="0"/>
-        <v>17.685117999999999</v>
-      </c>
-      <c r="N65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J66">
-        <v>4</v>
-      </c>
-      <c r="K66">
-        <v>226.45578</v>
-      </c>
-      <c r="L66">
-        <f t="shared" si="0"/>
-        <v>22.645578</v>
-      </c>
-      <c r="N66" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J67">
-        <v>8</v>
-      </c>
-      <c r="K67">
-        <v>217.8289</v>
-      </c>
-      <c r="L67">
-        <f t="shared" si="0"/>
-        <v>21.782890000000002</v>
-      </c>
-      <c r="N67" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J68">
-        <v>11</v>
-      </c>
-      <c r="K68">
-        <v>294.75198</v>
-      </c>
-      <c r="L68">
-        <f t="shared" si="0"/>
-        <v>29.475198000000002</v>
-      </c>
-      <c r="N68" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J69">
-        <v>15</v>
-      </c>
-      <c r="K69">
-        <v>299.06542999999999</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="0"/>
-        <v>29.906542999999999</v>
-      </c>
-      <c r="N69" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J70">
-        <v>19</v>
-      </c>
-      <c r="K70">
-        <v>308.41122000000001</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="0"/>
-        <v>30.841122000000002</v>
-      </c>
-      <c r="N70" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J71">
-        <v>22</v>
-      </c>
-      <c r="K71">
-        <v>331.41626000000002</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="0"/>
-        <v>33.141626000000002</v>
-      </c>
-      <c r="N71" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J72">
-        <v>25</v>
-      </c>
-      <c r="K72">
-        <v>390.36664000000002</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="0"/>
-        <v>39.036664000000002</v>
-      </c>
-      <c r="N72" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J73">
-        <v>30</v>
-      </c>
-      <c r="K73">
-        <v>462.97629999999998</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="0"/>
-        <v>46.297629999999998</v>
-      </c>
-      <c r="N73" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J74">
-        <v>33</v>
-      </c>
-      <c r="K74">
-        <v>539.89935000000003</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="0"/>
-        <v>53.989935000000003</v>
-      </c>
-      <c r="N74" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DF631D-DF5E-4A3F-BA90-F9B6EDEECD77}">
   <dimension ref="B1:G30"/>
   <sheetViews>
@@ -2506,35 +1700,35 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
@@ -2583,12 +1777,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d2997880b21379c034af171036c714b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc8da3ca17bc816b72b8261a93c82e58" ns2:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -2752,6 +1940,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
@@ -2761,23 +1955,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC49ADB-EC6A-4DF3-B319-3B0D82EDF8F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2793,4 +1970,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rewriting ParameterIdentification class to be independent of esqlabs
</commit_message>
<xml_diff>
--- a/tests/dev/Data/DataSet.xlsx
+++ b/tests/dev/Data/DataSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svavil\Downloads\esqlabs\OSPSuite.ParameterIdentification\tests\dev\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1B4625-C6ED-4C6F-A1BF-E5B994930148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580A26D3-7DF3-47E6-923A-44D3A4780EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="27">
   <si>
     <t>Study Id</t>
   </si>
@@ -1116,6 +1116,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
       <c r="J2">
         <v>1</v>
       </c>
@@ -1127,6 +1130,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
       <c r="J3">
         <v>4</v>
       </c>
@@ -1138,6 +1144,9 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
       <c r="J4">
         <v>8</v>
       </c>
@@ -1149,6 +1158,9 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
       <c r="J5">
         <v>11</v>
       </c>
@@ -1160,6 +1172,9 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
       <c r="J6">
         <v>15</v>
       </c>
@@ -1171,6 +1186,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
       <c r="J7">
         <v>19</v>
       </c>
@@ -1182,6 +1200,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
       <c r="J8">
         <v>22</v>
       </c>
@@ -1193,6 +1214,9 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
       <c r="J9">
         <v>25</v>
       </c>
@@ -1204,6 +1228,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
       <c r="J10">
         <v>30</v>
       </c>
@@ -1215,6 +1242,9 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
       <c r="J11">
         <v>33</v>
       </c>
@@ -1226,6 +1256,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
       <c r="J12">
         <v>1</v>
       </c>
@@ -1237,6 +1270,9 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
       <c r="J13">
         <v>4</v>
       </c>
@@ -1248,6 +1284,9 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
       <c r="J14">
         <v>8</v>
       </c>
@@ -1259,6 +1298,9 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
       <c r="J15">
         <v>11</v>
       </c>
@@ -1270,6 +1312,9 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
       <c r="J16">
         <v>15</v>
       </c>
@@ -1280,7 +1325,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
       <c r="J17">
         <v>19</v>
       </c>
@@ -1291,7 +1339,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
       <c r="J18">
         <v>22</v>
       </c>
@@ -1302,7 +1353,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
       <c r="J19">
         <v>25</v>
       </c>
@@ -1313,7 +1367,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
       <c r="J20">
         <v>30</v>
       </c>
@@ -1324,7 +1381,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
       <c r="J21">
         <v>33</v>
       </c>
@@ -1335,7 +1395,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
       <c r="J22">
         <v>1</v>
       </c>
@@ -1346,7 +1409,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
       <c r="J23">
         <v>4</v>
       </c>
@@ -1357,7 +1423,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
       <c r="J24">
         <v>8</v>
       </c>
@@ -1368,7 +1437,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
       <c r="J25">
         <v>11</v>
       </c>
@@ -1379,7 +1451,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
       <c r="J26">
         <v>15</v>
       </c>
@@ -1390,7 +1465,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
       <c r="J27">
         <v>19</v>
       </c>
@@ -1401,7 +1479,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
       <c r="J28">
         <v>22</v>
       </c>
@@ -1412,7 +1493,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
       <c r="J29">
         <v>25</v>
       </c>
@@ -1423,7 +1507,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
       <c r="J30">
         <v>30</v>
       </c>
@@ -1434,7 +1521,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
       <c r="J31">
         <v>33</v>
       </c>
@@ -1445,7 +1535,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
       <c r="J32">
         <v>1</v>
       </c>
@@ -1456,7 +1549,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
       <c r="J33">
         <v>4</v>
       </c>
@@ -1467,7 +1563,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
       <c r="J34">
         <v>8</v>
       </c>
@@ -1478,7 +1577,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
       <c r="J35">
         <v>11</v>
       </c>
@@ -1489,7 +1591,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
       <c r="J36">
         <v>15</v>
       </c>
@@ -1500,7 +1605,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
       <c r="J37">
         <v>19</v>
       </c>
@@ -1511,7 +1619,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
       <c r="J38">
         <v>22</v>
       </c>
@@ -1522,7 +1633,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
       <c r="J39">
         <v>25</v>
       </c>
@@ -1533,7 +1647,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
       <c r="J40">
         <v>30</v>
       </c>
@@ -1544,7 +1661,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
       <c r="J41">
         <v>33</v>
       </c>
@@ -1555,7 +1675,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
       <c r="J42">
         <v>1</v>
       </c>
@@ -1566,7 +1689,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
       <c r="J43">
         <v>4</v>
       </c>
@@ -1577,7 +1703,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
       <c r="J44">
         <v>8</v>
       </c>
@@ -1588,7 +1717,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
       <c r="J45">
         <v>11</v>
       </c>
@@ -1599,7 +1731,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
       <c r="J46">
         <v>15</v>
       </c>
@@ -1610,7 +1745,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
       <c r="J47">
         <v>19</v>
       </c>
@@ -1621,7 +1759,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
       <c r="J48">
         <v>22</v>
       </c>
@@ -1632,7 +1773,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
       <c r="J49">
         <v>25</v>
       </c>
@@ -1643,7 +1787,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
       <c r="J50">
         <v>30</v>
       </c>
@@ -1654,7 +1801,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
       <c r="J51">
         <v>33</v>
       </c>
@@ -1768,12 +1918,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1941,15 +2088,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1973,18 +2132,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Added new example - SteadyState completely commented out - Fixed some bugs in ParameterIdentification
</commit_message>
<xml_diff>
--- a/tests/dev/Data/DataSet.xlsx
+++ b/tests/dev/Data/DataSet.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite.ParameterIdentification\tests\dev\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F493C-4F71-43CB-A40F-8A4A4A16F484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BE972C-E93F-4221-9AB1-1B7400C0BE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="28800" windowHeight="18940" tabRatio="875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" tabRatio="875" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boswell_2012" sheetId="64" r:id="rId1"/>
     <sheet name="Boswell_2012_Error" sheetId="65" r:id="rId2"/>
-    <sheet name="MetaInfo" sheetId="48" r:id="rId3"/>
+    <sheet name="Backer_1989" sheetId="66" r:id="rId3"/>
+    <sheet name="McClain_1988" sheetId="67" r:id="rId4"/>
+    <sheet name="Marshall_1984" sheetId="68" r:id="rId5"/>
+    <sheet name="DoseResponse" sheetId="69" r:id="rId6"/>
+    <sheet name="Cedersund_2008" sheetId="70" r:id="rId7"/>
+    <sheet name="MetaInfo" sheetId="48" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="41">
   <si>
     <t>Study Id</t>
   </si>
@@ -180,6 +185,48 @@
   </si>
   <si>
     <t>MW</t>
+  </si>
+  <si>
+    <t>Time [min]</t>
+  </si>
+  <si>
+    <t>Fraction []</t>
+  </si>
+  <si>
+    <t>Error []</t>
+  </si>
+  <si>
+    <t>100 [nmol] insulin</t>
+  </si>
+  <si>
+    <t>IR_Int_Percent</t>
+  </si>
+  <si>
+    <t>IR_P_Percent</t>
+  </si>
+  <si>
+    <t>17.2 [nM] Insulin</t>
+  </si>
+  <si>
+    <t>Fraction [%]</t>
+  </si>
+  <si>
+    <t>Error [%]</t>
+  </si>
+  <si>
+    <t>IR_P_rel</t>
+  </si>
+  <si>
+    <t>IRS_P_rel</t>
+  </si>
+  <si>
+    <t>Dimensionless []</t>
+  </si>
+  <si>
+    <t>IRS_P</t>
+  </si>
+  <si>
+    <t>IR_P</t>
   </si>
 </sst>
 </file>
@@ -1066,13 +1113,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FB60DA-1FD0-45A2-84E9-D44628671A39}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:N51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>1</v>
       </c>
@@ -1127,7 +1179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>4</v>
       </c>
@@ -1138,7 +1190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>8</v>
       </c>
@@ -1149,7 +1201,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>11</v>
       </c>
@@ -1160,7 +1212,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>15</v>
       </c>
@@ -1171,7 +1223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>19</v>
       </c>
@@ -1182,7 +1234,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>22</v>
       </c>
@@ -1193,7 +1245,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>25</v>
       </c>
@@ -1204,7 +1256,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>30</v>
       </c>
@@ -1215,7 +1267,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>33</v>
       </c>
@@ -1226,7 +1278,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>1</v>
       </c>
@@ -1237,7 +1289,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>4</v>
       </c>
@@ -1248,7 +1300,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>8</v>
       </c>
@@ -1259,7 +1311,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>11</v>
       </c>
@@ -1270,7 +1322,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>15</v>
       </c>
@@ -1281,7 +1333,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>19</v>
       </c>
@@ -1292,7 +1344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>22</v>
       </c>
@@ -1303,7 +1355,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>25</v>
       </c>
@@ -1314,7 +1366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>30</v>
       </c>
@@ -1325,7 +1377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>33</v>
       </c>
@@ -1336,7 +1388,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>1</v>
       </c>
@@ -1347,7 +1399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>4</v>
       </c>
@@ -1358,7 +1410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>8</v>
       </c>
@@ -1369,7 +1421,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>11</v>
       </c>
@@ -1380,7 +1432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>15</v>
       </c>
@@ -1391,7 +1443,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>19</v>
       </c>
@@ -1402,7 +1454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>22</v>
       </c>
@@ -1413,7 +1465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>25</v>
       </c>
@@ -1424,7 +1476,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>30</v>
       </c>
@@ -1435,7 +1487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>33</v>
       </c>
@@ -1446,7 +1498,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>1</v>
       </c>
@@ -1457,7 +1509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>4</v>
       </c>
@@ -1468,7 +1520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>8</v>
       </c>
@@ -1479,7 +1531,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>11</v>
       </c>
@@ -1490,7 +1542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>15</v>
       </c>
@@ -1501,7 +1553,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>19</v>
       </c>
@@ -1512,7 +1564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>22</v>
       </c>
@@ -1523,7 +1575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>25</v>
       </c>
@@ -1534,7 +1586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>30</v>
       </c>
@@ -1545,7 +1597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>33</v>
       </c>
@@ -1556,7 +1608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>1</v>
       </c>
@@ -1567,7 +1619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>4</v>
       </c>
@@ -1578,7 +1630,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>8</v>
       </c>
@@ -1589,7 +1641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>11</v>
       </c>
@@ -1600,7 +1652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>15</v>
       </c>
@@ -1611,7 +1663,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>19</v>
       </c>
@@ -1622,7 +1674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>22</v>
       </c>
@@ -1633,7 +1685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>25</v>
       </c>
@@ -1644,7 +1696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>30</v>
       </c>
@@ -1655,7 +1707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>33</v>
       </c>
@@ -1673,805 +1725,805 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E130360-29C4-4F79-90A7-EBE9DBEF9F87}">
-  <dimension ref="A24:N74"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25:L74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>176.85118</v>
+      </c>
+      <c r="L2">
+        <f>K2*0.1</f>
+        <v>17.685117999999999</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>219.98562999999999</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L51" si="0">K3*0.1</f>
+        <v>21.998563000000001</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>263.12006000000002</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>26.312006000000004</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5">
+        <v>331.41626000000002</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>33.141626000000002</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>385.33429999999998</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>38.533430000000003</v>
+      </c>
+      <c r="N6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J7">
+        <v>19</v>
+      </c>
+      <c r="K7">
+        <v>431.34435999999999</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>43.134436000000001</v>
+      </c>
+      <c r="N7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J8">
+        <v>22</v>
+      </c>
+      <c r="K8">
+        <v>524.08339999999998</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>52.408340000000003</v>
+      </c>
+      <c r="N8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J9">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>561.46654999999998</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>56.146655000000003</v>
+      </c>
+      <c r="N9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J10">
+        <v>30</v>
+      </c>
+      <c r="K10">
+        <v>647.01653999999996</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>64.701654000000005</v>
+      </c>
+      <c r="N10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J11">
+        <v>33</v>
+      </c>
+      <c r="K11">
+        <v>706.68584999999996</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>70.668584999999993</v>
+      </c>
+      <c r="N11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>173.25665000000001</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>17.325665000000001</v>
+      </c>
+      <c r="N12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>251.61753999999999</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>25.161754000000002</v>
+      </c>
+      <c r="N13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>224.29907</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>22.429907</v>
+      </c>
+      <c r="N14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J15">
+        <v>11</v>
+      </c>
+      <c r="K15">
+        <v>282.53055000000001</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>28.253055000000003</v>
+      </c>
+      <c r="N15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <v>334.29187000000002</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>33.429187000000006</v>
+      </c>
+      <c r="N16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J17">
+        <v>19</v>
+      </c>
+      <c r="K17">
+        <v>360.17255</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>36.017254999999999</v>
+      </c>
+      <c r="N17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J18">
+        <v>22</v>
+      </c>
+      <c r="K18">
+        <v>405.46368000000001</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>40.546368000000001</v>
+      </c>
+      <c r="N18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J19">
+        <v>25</v>
+      </c>
+      <c r="K19">
+        <v>512.58090000000004</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>51.25809000000001</v>
+      </c>
+      <c r="N19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J20">
+        <v>30</v>
+      </c>
+      <c r="K20">
+        <v>588.78503000000001</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>58.878503000000002</v>
+      </c>
+      <c r="N20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J21">
+        <v>33</v>
+      </c>
+      <c r="K21">
+        <v>693.02660000000003</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>69.302660000000003</v>
+      </c>
+      <c r="N21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>168.94319999999999</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>16.89432</v>
+      </c>
+      <c r="N22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <v>214.95328000000001</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>21.495328000000001</v>
+      </c>
+      <c r="N23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J24">
+        <v>8</v>
+      </c>
+      <c r="K24">
+        <v>224.29907</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>22.429907</v>
+      </c>
+      <c r="N24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
+        <v>11</v>
+      </c>
+      <c r="K25">
+        <v>269.59019999999998</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>26.959019999999999</v>
+      </c>
+      <c r="N25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J26">
+        <v>15</v>
+      </c>
+      <c r="K26">
+        <v>306.97340000000003</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>30.697340000000004</v>
+      </c>
+      <c r="N26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J27">
+        <v>19</v>
+      </c>
+      <c r="K27">
+        <v>352.98345999999998</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>35.298346000000002</v>
+      </c>
+      <c r="N27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J28">
+        <v>22</v>
+      </c>
+      <c r="K28">
+        <v>407.62042000000002</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>40.762042000000008</v>
+      </c>
+      <c r="N28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J29">
+        <v>25</v>
+      </c>
+      <c r="K29">
+        <v>483.82459999999998</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>48.382460000000002</v>
+      </c>
+      <c r="N29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J30">
+        <v>30</v>
+      </c>
+      <c r="K30">
+        <v>610.35230000000001</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>61.035230000000006</v>
+      </c>
+      <c r="N30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J31">
+        <v>33</v>
+      </c>
+      <c r="K31">
+        <v>683.68079999999998</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>68.368080000000006</v>
+      </c>
+      <c r="N31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J32">
         <v>1</v>
       </c>
-      <c r="K25">
+      <c r="K32">
+        <v>173.25665000000001</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>17.325665000000001</v>
+      </c>
+      <c r="N32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>231.48813999999999</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>23.148814000000002</v>
+      </c>
+      <c r="N33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J34">
+        <v>8</v>
+      </c>
+      <c r="K34">
+        <v>178.28899999999999</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>17.828900000000001</v>
+      </c>
+      <c r="N34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J35">
+        <v>11</v>
+      </c>
+      <c r="K35">
+        <v>242.27173999999999</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>24.227174000000002</v>
+      </c>
+      <c r="N35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J36">
+        <v>15</v>
+      </c>
+      <c r="K36">
+        <v>264.55786000000001</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>26.455786000000003</v>
+      </c>
+      <c r="N36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J37">
+        <v>19</v>
+      </c>
+      <c r="K37">
+        <v>268.1524</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>26.815240000000003</v>
+      </c>
+      <c r="N37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J38">
+        <v>22</v>
+      </c>
+      <c r="K38">
+        <v>291.87634000000003</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="0"/>
+        <v>29.187634000000003</v>
+      </c>
+      <c r="N38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J39">
+        <v>25</v>
+      </c>
+      <c r="K39">
+        <v>322.07047</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>32.207047000000003</v>
+      </c>
+      <c r="N39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J40">
+        <v>30</v>
+      </c>
+      <c r="K40">
+        <v>443.56576999999999</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>44.356577000000001</v>
+      </c>
+      <c r="N40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J41">
+        <v>33</v>
+      </c>
+      <c r="K41">
+        <v>516.89435000000003</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>51.689435000000003</v>
+      </c>
+      <c r="N41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
         <v>176.85118</v>
       </c>
-      <c r="L25">
-        <f>K25*0.1</f>
+      <c r="L42">
+        <f t="shared" si="0"/>
         <v>17.685117999999999</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J43">
+        <v>4</v>
+      </c>
+      <c r="K43">
+        <v>226.45578</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>22.645578</v>
+      </c>
+      <c r="N43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J44">
+        <v>8</v>
+      </c>
+      <c r="K44">
+        <v>217.8289</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>21.782890000000002</v>
+      </c>
+      <c r="N44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J45">
+        <v>11</v>
+      </c>
+      <c r="K45">
+        <v>294.75198</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>29.475198000000002</v>
+      </c>
+      <c r="N45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J46">
+        <v>15</v>
+      </c>
+      <c r="K46">
+        <v>299.06542999999999</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>29.906542999999999</v>
+      </c>
+      <c r="N46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J47">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J26">
-        <v>4</v>
-      </c>
-      <c r="K26">
-        <v>219.98562999999999</v>
-      </c>
-      <c r="L26">
-        <f t="shared" ref="L26:L74" si="0">K26*0.1</f>
-        <v>21.998563000000001</v>
-      </c>
-      <c r="N26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J27">
-        <v>8</v>
-      </c>
-      <c r="K27">
-        <v>263.12006000000002</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
-        <v>26.312006000000004</v>
-      </c>
-      <c r="N27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J28">
-        <v>11</v>
-      </c>
-      <c r="K28">
+      <c r="K47">
+        <v>308.41122000000001</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>30.841122000000002</v>
+      </c>
+      <c r="N47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J48">
+        <v>22</v>
+      </c>
+      <c r="K48">
         <v>331.41626000000002</v>
       </c>
-      <c r="L28">
+      <c r="L48">
         <f t="shared" si="0"/>
         <v>33.141626000000002</v>
       </c>
-      <c r="N28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J29">
-        <v>15</v>
-      </c>
-      <c r="K29">
-        <v>385.33429999999998</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="0"/>
-        <v>38.533430000000003</v>
-      </c>
-      <c r="N29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J30">
-        <v>19</v>
-      </c>
-      <c r="K30">
-        <v>431.34435999999999</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="0"/>
-        <v>43.134436000000001</v>
-      </c>
-      <c r="N30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J31">
-        <v>22</v>
-      </c>
-      <c r="K31">
-        <v>524.08339999999998</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
-        <v>52.408340000000003</v>
-      </c>
-      <c r="N31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J32">
+      <c r="N48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J49">
         <v>25</v>
       </c>
-      <c r="K32">
-        <v>561.46654999999998</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="0"/>
-        <v>56.146655000000003</v>
-      </c>
-      <c r="N32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J33">
+      <c r="K49">
+        <v>390.36664000000002</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>39.036664000000002</v>
+      </c>
+      <c r="N49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J50">
         <v>30</v>
       </c>
-      <c r="K33">
-        <v>647.01653999999996</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="0"/>
-        <v>64.701654000000005</v>
-      </c>
-      <c r="N33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J34">
+      <c r="K50">
+        <v>462.97629999999998</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="0"/>
+        <v>46.297629999999998</v>
+      </c>
+      <c r="N50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J51">
         <v>33</v>
       </c>
-      <c r="K34">
-        <v>706.68584999999996</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="0"/>
-        <v>70.668584999999993</v>
-      </c>
-      <c r="N34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="K35">
-        <v>173.25665000000001</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="0"/>
-        <v>17.325665000000001</v>
-      </c>
-      <c r="N35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J36">
-        <v>4</v>
-      </c>
-      <c r="K36">
-        <v>251.61753999999999</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="0"/>
-        <v>25.161754000000002</v>
-      </c>
-      <c r="N36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J37">
-        <v>8</v>
-      </c>
-      <c r="K37">
-        <v>224.29907</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="0"/>
-        <v>22.429907</v>
-      </c>
-      <c r="N37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J38">
-        <v>11</v>
-      </c>
-      <c r="K38">
-        <v>282.53055000000001</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="0"/>
-        <v>28.253055000000003</v>
-      </c>
-      <c r="N38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J39">
-        <v>15</v>
-      </c>
-      <c r="K39">
-        <v>334.29187000000002</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="0"/>
-        <v>33.429187000000006</v>
-      </c>
-      <c r="N39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J40">
-        <v>19</v>
-      </c>
-      <c r="K40">
-        <v>360.17255</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="0"/>
-        <v>36.017254999999999</v>
-      </c>
-      <c r="N40" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J41">
-        <v>22</v>
-      </c>
-      <c r="K41">
-        <v>405.46368000000001</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="0"/>
-        <v>40.546368000000001</v>
-      </c>
-      <c r="N41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J42">
-        <v>25</v>
-      </c>
-      <c r="K42">
-        <v>512.58090000000004</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="0"/>
-        <v>51.25809000000001</v>
-      </c>
-      <c r="N42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J43">
-        <v>30</v>
-      </c>
-      <c r="K43">
-        <v>588.78503000000001</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="0"/>
-        <v>58.878503000000002</v>
-      </c>
-      <c r="N43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J44">
-        <v>33</v>
-      </c>
-      <c r="K44">
-        <v>693.02660000000003</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="0"/>
-        <v>69.302660000000003</v>
-      </c>
-      <c r="N44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J45">
-        <v>1</v>
-      </c>
-      <c r="K45">
-        <v>168.94319999999999</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="0"/>
-        <v>16.89432</v>
-      </c>
-      <c r="N45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J46">
-        <v>4</v>
-      </c>
-      <c r="K46">
-        <v>214.95328000000001</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="0"/>
-        <v>21.495328000000001</v>
-      </c>
-      <c r="N46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J47">
-        <v>8</v>
-      </c>
-      <c r="K47">
-        <v>224.29907</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="0"/>
-        <v>22.429907</v>
-      </c>
-      <c r="N47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J48">
-        <v>11</v>
-      </c>
-      <c r="K48">
-        <v>269.59019999999998</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="0"/>
-        <v>26.959019999999999</v>
-      </c>
-      <c r="N48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J49">
-        <v>15</v>
-      </c>
-      <c r="K49">
-        <v>306.97340000000003</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="0"/>
-        <v>30.697340000000004</v>
-      </c>
-      <c r="N49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J50">
-        <v>19</v>
-      </c>
-      <c r="K50">
-        <v>352.98345999999998</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="0"/>
-        <v>35.298346000000002</v>
-      </c>
-      <c r="N50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J51">
-        <v>22</v>
-      </c>
       <c r="K51">
-        <v>407.62042000000002</v>
+        <v>539.89935000000003</v>
       </c>
       <c r="L51">
         <f t="shared" si="0"/>
-        <v>40.762042000000008</v>
+        <v>53.989935000000003</v>
       </c>
       <c r="N51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J52">
-        <v>25</v>
-      </c>
-      <c r="K52">
-        <v>483.82459999999998</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
-        <v>48.382460000000002</v>
-      </c>
-      <c r="N52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J53">
-        <v>30</v>
-      </c>
-      <c r="K53">
-        <v>610.35230000000001</v>
-      </c>
-      <c r="L53">
-        <f t="shared" si="0"/>
-        <v>61.035230000000006</v>
-      </c>
-      <c r="N53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J54">
-        <v>33</v>
-      </c>
-      <c r="K54">
-        <v>683.68079999999998</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="0"/>
-        <v>68.368080000000006</v>
-      </c>
-      <c r="N54" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J55">
-        <v>1</v>
-      </c>
-      <c r="K55">
-        <v>173.25665000000001</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="0"/>
-        <v>17.325665000000001</v>
-      </c>
-      <c r="N55" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J56">
-        <v>4</v>
-      </c>
-      <c r="K56">
-        <v>231.48813999999999</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="0"/>
-        <v>23.148814000000002</v>
-      </c>
-      <c r="N56" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J57">
-        <v>8</v>
-      </c>
-      <c r="K57">
-        <v>178.28899999999999</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
-        <v>17.828900000000001</v>
-      </c>
-      <c r="N57" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J58">
-        <v>11</v>
-      </c>
-      <c r="K58">
-        <v>242.27173999999999</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="0"/>
-        <v>24.227174000000002</v>
-      </c>
-      <c r="N58" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J59">
-        <v>15</v>
-      </c>
-      <c r="K59">
-        <v>264.55786000000001</v>
-      </c>
-      <c r="L59">
-        <f t="shared" si="0"/>
-        <v>26.455786000000003</v>
-      </c>
-      <c r="N59" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J60">
-        <v>19</v>
-      </c>
-      <c r="K60">
-        <v>268.1524</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="0"/>
-        <v>26.815240000000003</v>
-      </c>
-      <c r="N60" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J61">
-        <v>22</v>
-      </c>
-      <c r="K61">
-        <v>291.87634000000003</v>
-      </c>
-      <c r="L61">
-        <f t="shared" si="0"/>
-        <v>29.187634000000003</v>
-      </c>
-      <c r="N61" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J62">
-        <v>25</v>
-      </c>
-      <c r="K62">
-        <v>322.07047</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="0"/>
-        <v>32.207047000000003</v>
-      </c>
-      <c r="N62" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J63">
-        <v>30</v>
-      </c>
-      <c r="K63">
-        <v>443.56576999999999</v>
-      </c>
-      <c r="L63">
-        <f t="shared" si="0"/>
-        <v>44.356577000000001</v>
-      </c>
-      <c r="N63" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J64">
-        <v>33</v>
-      </c>
-      <c r="K64">
-        <v>516.89435000000003</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="0"/>
-        <v>51.689435000000003</v>
-      </c>
-      <c r="N64" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J65">
-        <v>1</v>
-      </c>
-      <c r="K65">
-        <v>176.85118</v>
-      </c>
-      <c r="L65">
-        <f t="shared" si="0"/>
-        <v>17.685117999999999</v>
-      </c>
-      <c r="N65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J66">
-        <v>4</v>
-      </c>
-      <c r="K66">
-        <v>226.45578</v>
-      </c>
-      <c r="L66">
-        <f t="shared" si="0"/>
-        <v>22.645578</v>
-      </c>
-      <c r="N66" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J67">
-        <v>8</v>
-      </c>
-      <c r="K67">
-        <v>217.8289</v>
-      </c>
-      <c r="L67">
-        <f t="shared" si="0"/>
-        <v>21.782890000000002</v>
-      </c>
-      <c r="N67" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J68">
-        <v>11</v>
-      </c>
-      <c r="K68">
-        <v>294.75198</v>
-      </c>
-      <c r="L68">
-        <f t="shared" si="0"/>
-        <v>29.475198000000002</v>
-      </c>
-      <c r="N68" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J69">
-        <v>15</v>
-      </c>
-      <c r="K69">
-        <v>299.06542999999999</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="0"/>
-        <v>29.906542999999999</v>
-      </c>
-      <c r="N69" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J70">
-        <v>19</v>
-      </c>
-      <c r="K70">
-        <v>308.41122000000001</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="0"/>
-        <v>30.841122000000002</v>
-      </c>
-      <c r="N70" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J71">
-        <v>22</v>
-      </c>
-      <c r="K71">
-        <v>331.41626000000002</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="0"/>
-        <v>33.141626000000002</v>
-      </c>
-      <c r="N71" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J72">
-        <v>25</v>
-      </c>
-      <c r="K72">
-        <v>390.36664000000002</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="0"/>
-        <v>39.036664000000002</v>
-      </c>
-      <c r="N72" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J73">
-        <v>30</v>
-      </c>
-      <c r="K73">
-        <v>462.97629999999998</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="0"/>
-        <v>46.297629999999998</v>
-      </c>
-      <c r="N73" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
-      <c r="J74">
-        <v>33</v>
-      </c>
-      <c r="K74">
-        <v>539.89935000000003</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="0"/>
-        <v>53.989935000000003</v>
-      </c>
-      <c r="N74" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2481,6 +2533,1238 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6600E2ED-F2AE-45A7-9FDF-BFC50F5317AB}">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.73046875" customWidth="1"/>
+    <col min="10" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2">
+        <v>1.97137548367323</v>
+      </c>
+      <c r="K2">
+        <v>5.9562044261688006E-2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3">
+        <v>5.2484771476368604</v>
+      </c>
+      <c r="K3">
+        <v>0.125992886970513</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <v>9.6900340965686294</v>
+      </c>
+      <c r="K4">
+        <v>0.21059260347095399</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <v>15.023465335155199</v>
+      </c>
+      <c r="K5">
+        <v>0.27258897671983301</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>20.358907888183602</v>
+      </c>
+      <c r="K6">
+        <v>0.33646736562503898</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7">
+        <v>30.335314850524199</v>
+      </c>
+      <c r="K7">
+        <v>0.38581959467225097</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>45.150178144993397</v>
+      </c>
+      <c r="K8">
+        <v>0.39115596306843498</v>
+      </c>
+      <c r="N8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <v>60.824160036778302</v>
+      </c>
+      <c r="K9">
+        <v>0.41466759038144702</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10">
+        <v>70</v>
+      </c>
+      <c r="K10">
+        <v>0.19407067763684099</v>
+      </c>
+      <c r="N10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11">
+        <v>74.866729516626663</v>
+      </c>
+      <c r="K11">
+        <v>0.15582219174951401</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12">
+        <v>79.822306022168888</v>
+      </c>
+      <c r="K12">
+        <v>6.3537976612196706E-2</v>
+      </c>
+      <c r="N12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13">
+        <v>90.137127185464493</v>
+      </c>
+      <c r="K13">
+        <v>1.1751514112672801E-2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14">
+        <v>100.0214261227288</v>
+      </c>
+      <c r="K14">
+        <v>1.1697234601759801E-2</v>
+      </c>
+      <c r="N14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15">
+        <v>115.4075248543023</v>
+      </c>
+      <c r="K15">
+        <v>3.4347503142498001E-2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16">
+        <v>130.26068449320081</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED695098-43E4-4244-8496-0C9DFC0CC5D4}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="9" max="9" width="12.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2">
+        <v>30.005079736123442</v>
+      </c>
+      <c r="K2">
+        <v>0.16633663366336598</v>
+      </c>
+      <c r="L2">
+        <v>3.712871287129005E-3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <v>30.971915352715747</v>
+      </c>
+      <c r="K3">
+        <v>0.308168316831683</v>
+      </c>
+      <c r="L3">
+        <v>8.9108910891090073E-3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <v>32.0126993403086</v>
+      </c>
+      <c r="K4">
+        <v>0.49306930693069301</v>
+      </c>
+      <c r="L4">
+        <v>2.227722772277204E-2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5">
+        <v>33.993773951742497</v>
+      </c>
+      <c r="K5">
+        <v>0.54282178217821708</v>
+      </c>
+      <c r="L5">
+        <v>2.1534653465346949E-2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>38.008383812274531</v>
+      </c>
+      <c r="K6">
+        <v>0.57549504950495001</v>
+      </c>
+      <c r="L6">
+        <v>1.3366336633662997E-2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7">
+        <v>45.981906249648802</v>
+      </c>
+      <c r="K7">
+        <v>0.60074257425742505</v>
+      </c>
+      <c r="L7">
+        <v>3.7871287128713009E-2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185B249F-217F-4EA7-8E94-E45F0BCB0F43}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>0.1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <v>30.418764464328309</v>
+      </c>
+      <c r="K3">
+        <v>0.14722656182938781</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <v>30.936289267226652</v>
+      </c>
+      <c r="K4">
+        <v>0.15218287009219073</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5">
+        <v>31.467416179418912</v>
+      </c>
+      <c r="K5">
+        <v>0.22059606173496588</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>31.947938087839969</v>
+      </c>
+      <c r="K6">
+        <v>0.24476986729385974</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7">
+        <v>32.976927986178708</v>
+      </c>
+      <c r="K7">
+        <v>0.3450531339593812</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8">
+        <v>34.008432018462763</v>
+      </c>
+      <c r="K8">
+        <v>0.4078421947157902</v>
+      </c>
+      <c r="N8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9">
+        <v>35.963719113219831</v>
+      </c>
+      <c r="K9">
+        <v>0.54204192346649882</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10">
+        <v>38.036074598866698</v>
+      </c>
+      <c r="K10">
+        <v>0.52821851018901522</v>
+      </c>
+      <c r="N10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11">
+        <v>39.947525512013044</v>
+      </c>
+      <c r="K11">
+        <v>0.51723291386976722</v>
+      </c>
+      <c r="N11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A857DC-3FB6-40E0-B0A3-FE498C8662D5}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J3">
+        <v>30</v>
+      </c>
+      <c r="K3">
+        <v>4.3267998695373535</v>
+      </c>
+      <c r="L3">
+        <v>1.9299999475479126</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>20.090000152587891</v>
+      </c>
+      <c r="L4">
+        <v>8.5299997329711914</v>
+      </c>
+      <c r="N4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J5">
+        <v>70</v>
+      </c>
+      <c r="K5">
+        <v>26.440000534057617</v>
+      </c>
+      <c r="L5">
+        <v>9.2299995422363281</v>
+      </c>
+      <c r="N5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J6">
+        <v>90</v>
+      </c>
+      <c r="K6">
+        <v>47.380001068115234</v>
+      </c>
+      <c r="L6">
+        <v>10.079999923706055</v>
+      </c>
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J7">
+        <v>110</v>
+      </c>
+      <c r="K7">
+        <v>88.449996948242188</v>
+      </c>
+      <c r="L7">
+        <v>3.0399999618530273</v>
+      </c>
+      <c r="N7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J8">
+        <v>130</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>0.62000000476837158</v>
+      </c>
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J10">
+        <v>30</v>
+      </c>
+      <c r="K10">
+        <v>20.399999618530273</v>
+      </c>
+      <c r="L10">
+        <v>9.5699996948242188</v>
+      </c>
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11">
+        <v>29.899999618530273</v>
+      </c>
+      <c r="L11">
+        <v>7.2199997901916504</v>
+      </c>
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J12">
+        <v>70</v>
+      </c>
+      <c r="K12">
+        <v>49.900001525878906</v>
+      </c>
+      <c r="L12">
+        <v>7.7100000381469727</v>
+      </c>
+      <c r="N12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J13">
+        <v>90</v>
+      </c>
+      <c r="K13">
+        <v>80.900001525878906</v>
+      </c>
+      <c r="L13">
+        <v>7.880000114440918</v>
+      </c>
+      <c r="N13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J14">
+        <v>110</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>6.2899999618530273</v>
+      </c>
+      <c r="N14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J15">
+        <v>130</v>
+      </c>
+      <c r="K15">
+        <v>90.099998474121094</v>
+      </c>
+      <c r="L15">
+        <v>8.5299997329711914</v>
+      </c>
+      <c r="N15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E64E9D-7A37-4C44-ABC1-67E774D19884}">
+  <dimension ref="A1:N19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="10" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J2">
+        <v>30.913095474243164</v>
+      </c>
+      <c r="K2">
+        <v>222.21975708007813</v>
+      </c>
+      <c r="L2">
+        <v>14.598901748657227</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J3">
+        <v>31.199090957641602</v>
+      </c>
+      <c r="K3">
+        <v>202.87785339355469</v>
+      </c>
+      <c r="L3">
+        <v>44.141326904296875</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J4">
+        <v>31.292362213134766</v>
+      </c>
+      <c r="K4">
+        <v>170.62400817871094</v>
+      </c>
+      <c r="L4">
+        <v>9.8508501052856445</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J5">
+        <v>32.328723907470703</v>
+      </c>
+      <c r="K5">
+        <v>145.88314819335938</v>
+      </c>
+      <c r="L5">
+        <v>8.4889945983886719</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J6">
+        <v>33.317161560058594</v>
+      </c>
+      <c r="K6">
+        <v>121.14013671875</v>
+      </c>
+      <c r="L6">
+        <v>26.819438934326172</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J7">
+        <v>35.361003875732422</v>
+      </c>
+      <c r="K7">
+        <v>110.02722930908203</v>
+      </c>
+      <c r="L7">
+        <v>24.783525466918945</v>
+      </c>
+      <c r="N7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J8">
+        <v>37.021049499511719</v>
+      </c>
+      <c r="K8">
+        <v>93.803573608398438</v>
+      </c>
+      <c r="L8">
+        <v>28.190696716308594</v>
+      </c>
+      <c r="N8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J9">
+        <v>40.057559967041016</v>
+      </c>
+      <c r="K9">
+        <v>110.91898345947266</v>
+      </c>
+      <c r="L9">
+        <v>13.250787734985352</v>
+      </c>
+      <c r="N9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J10">
+        <v>45.023651123046875</v>
+      </c>
+      <c r="K10">
+        <v>86.356040954589844</v>
+      </c>
+      <c r="L10">
+        <v>33.945133209228516</v>
+      </c>
+      <c r="N10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J11">
+        <v>30.938276290893555</v>
+      </c>
+      <c r="K11">
+        <v>100.65204620361328</v>
+      </c>
+      <c r="L11">
+        <v>9.5635957717895508</v>
+      </c>
+      <c r="N11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J12">
+        <v>31.350343704223633</v>
+      </c>
+      <c r="K12">
+        <v>85.273147583007813</v>
+      </c>
+      <c r="L12">
+        <v>21.827781677246094</v>
+      </c>
+      <c r="N12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J13">
+        <v>31.660545349121094</v>
+      </c>
+      <c r="K13">
+        <v>78.416740417480469</v>
+      </c>
+      <c r="L13">
+        <v>18.917652130126953</v>
+      </c>
+      <c r="N13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J14">
+        <v>33.103797912597656</v>
+      </c>
+      <c r="K14">
+        <v>60.973121643066406</v>
+      </c>
+      <c r="L14">
+        <v>7.6925868988037109</v>
+      </c>
+      <c r="N14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J15">
+        <v>34.686233520507813</v>
+      </c>
+      <c r="K15">
+        <v>51.223747253417969</v>
+      </c>
+      <c r="L15">
+        <v>3.3275585174560547</v>
+      </c>
+      <c r="N15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="J16">
+        <v>37.690589904785156</v>
+      </c>
+      <c r="K16">
+        <v>56.670791625976563</v>
+      </c>
+      <c r="L16">
+        <v>15.591413497924805</v>
+      </c>
+      <c r="N16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J17">
+        <v>40.324306488037109</v>
+      </c>
+      <c r="K17">
+        <v>45.896484375</v>
+      </c>
+      <c r="L17">
+        <v>6.2363677024841309</v>
+      </c>
+      <c r="N17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J18">
+        <v>44.778003692626953</v>
+      </c>
+      <c r="K18">
+        <v>52.195217132568359</v>
+      </c>
+      <c r="L18">
+        <v>4.3656883239746094</v>
+      </c>
+      <c r="N18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J19">
+        <v>52.317726135253906</v>
+      </c>
+      <c r="K19">
+        <v>41.073108673095703</v>
+      </c>
+      <c r="L19">
+        <v>5.197577953338623</v>
+      </c>
+      <c r="N19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DF631D-DF5E-4A3F-BA90-F9B6EDEECD77}">
   <dimension ref="B1:G30"/>
   <sheetViews>
@@ -2488,23 +3772,23 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.54296875" style="2"/>
+    <col min="1" max="1" width="12.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.46484375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.53125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.46484375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.53125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2515,7 +3799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2526,7 +3810,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
@@ -2537,31 +3821,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C8" s="3"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C14" s="3"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D20" s="5"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D30" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update piTest to use DataSet
</commit_message>
<xml_diff>
--- a/tests/dev/Data/DataSet.xlsx
+++ b/tests/dev/Data/DataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite.ParameterIdentification\tests\dev\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8015C633-0F9D-428B-A61E-B0EBF7AE656D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ACDC6C-BC50-43D7-817E-CFDB6068B953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="720" windowWidth="38400" windowHeight="20505" tabRatio="875" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boswell_2012" sheetId="64" r:id="rId1"/>
@@ -207,9 +207,6 @@
     <t>Time unit</t>
   </si>
   <si>
-    <t>day[s]</t>
-  </si>
-  <si>
     <t>Measurement</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>day(s)</t>
   </si>
 </sst>
 </file>
@@ -772,10 +772,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1134,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FB60DA-1FD0-45A2-84E9-D44628671A39}">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,17 +1193,17 @@
       <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>6</v>
@@ -1212,16 +1212,16 @@
         <v>7</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1229,13 +1229,13 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L2">
         <v>176.85118</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N2">
         <v>17.685117999999999</v>
@@ -1249,13 +1249,13 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L3">
         <v>219.98562999999999</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N3">
         <v>21.998563000000001</v>
@@ -1269,13 +1269,13 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L4">
         <v>263.12006000000002</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N4">
         <v>26.312006000000004</v>
@@ -1289,13 +1289,13 @@
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L5">
         <v>331.41626000000002</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N5">
         <v>33.141626000000002</v>
@@ -1309,13 +1309,13 @@
         <v>15</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L6">
         <v>385.33429999999998</v>
       </c>
       <c r="M6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N6">
         <v>38.533430000000003</v>
@@ -1329,13 +1329,13 @@
         <v>19</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L7">
         <v>431.34435999999999</v>
       </c>
       <c r="M7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N7">
         <v>43.134436000000001</v>
@@ -1349,13 +1349,13 @@
         <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L8">
         <v>524.08339999999998</v>
       </c>
       <c r="M8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N8">
         <v>52.408340000000003</v>
@@ -1369,13 +1369,13 @@
         <v>25</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L9">
         <v>561.46654999999998</v>
       </c>
       <c r="M9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N9">
         <v>56.146655000000003</v>
@@ -1389,13 +1389,13 @@
         <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L10">
         <v>647.01653999999996</v>
       </c>
       <c r="M10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N10">
         <v>64.701654000000005</v>
@@ -1409,13 +1409,13 @@
         <v>33</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L11">
         <v>706.68584999999996</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N11">
         <v>70.668584999999993</v>
@@ -1429,13 +1429,13 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L12">
         <v>173.25665000000001</v>
       </c>
       <c r="M12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N12">
         <v>17.325665000000001</v>
@@ -1449,13 +1449,13 @@
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L13">
         <v>251.61753999999999</v>
       </c>
       <c r="M13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N13">
         <v>25.161754000000002</v>
@@ -1469,13 +1469,13 @@
         <v>8</v>
       </c>
       <c r="K14" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L14">
         <v>224.29907</v>
       </c>
       <c r="M14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N14">
         <v>22.429907</v>
@@ -1489,13 +1489,13 @@
         <v>11</v>
       </c>
       <c r="K15" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L15">
         <v>282.53055000000001</v>
       </c>
       <c r="M15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N15">
         <v>28.253055000000003</v>
@@ -1509,13 +1509,13 @@
         <v>15</v>
       </c>
       <c r="K16" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L16">
         <v>334.29187000000002</v>
       </c>
       <c r="M16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N16">
         <v>33.429187000000006</v>
@@ -1529,13 +1529,13 @@
         <v>19</v>
       </c>
       <c r="K17" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L17">
         <v>360.17255</v>
       </c>
       <c r="M17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N17">
         <v>36.017254999999999</v>
@@ -1549,13 +1549,13 @@
         <v>22</v>
       </c>
       <c r="K18" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L18">
         <v>405.46368000000001</v>
       </c>
       <c r="M18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N18">
         <v>40.546368000000001</v>
@@ -1569,13 +1569,13 @@
         <v>25</v>
       </c>
       <c r="K19" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L19">
         <v>512.58090000000004</v>
       </c>
       <c r="M19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N19">
         <v>51.25809000000001</v>
@@ -1589,13 +1589,13 @@
         <v>30</v>
       </c>
       <c r="K20" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L20">
         <v>588.78503000000001</v>
       </c>
       <c r="M20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N20">
         <v>58.878503000000002</v>
@@ -1609,13 +1609,13 @@
         <v>33</v>
       </c>
       <c r="K21" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L21">
         <v>693.02660000000003</v>
       </c>
       <c r="M21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N21">
         <v>69.302660000000003</v>
@@ -1629,13 +1629,13 @@
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L22">
         <v>168.94319999999999</v>
       </c>
       <c r="M22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N22">
         <v>16.89432</v>
@@ -1649,13 +1649,13 @@
         <v>4</v>
       </c>
       <c r="K23" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L23">
         <v>214.95328000000001</v>
       </c>
       <c r="M23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N23">
         <v>21.495328000000001</v>
@@ -1669,13 +1669,13 @@
         <v>8</v>
       </c>
       <c r="K24" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L24">
         <v>224.29907</v>
       </c>
       <c r="M24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N24">
         <v>22.429907</v>
@@ -1689,13 +1689,13 @@
         <v>11</v>
       </c>
       <c r="K25" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L25">
         <v>269.59019999999998</v>
       </c>
       <c r="M25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N25">
         <v>26.959019999999999</v>
@@ -1709,13 +1709,13 @@
         <v>15</v>
       </c>
       <c r="K26" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L26">
         <v>306.97340000000003</v>
       </c>
       <c r="M26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N26">
         <v>30.697340000000004</v>
@@ -1729,13 +1729,13 @@
         <v>19</v>
       </c>
       <c r="K27" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L27">
         <v>352.98345999999998</v>
       </c>
       <c r="M27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N27">
         <v>35.298346000000002</v>
@@ -1749,13 +1749,13 @@
         <v>22</v>
       </c>
       <c r="K28" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L28">
         <v>407.62042000000002</v>
       </c>
       <c r="M28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N28">
         <v>40.762042000000008</v>
@@ -1769,13 +1769,13 @@
         <v>25</v>
       </c>
       <c r="K29" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L29">
         <v>483.82459999999998</v>
       </c>
       <c r="M29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N29">
         <v>48.382460000000002</v>
@@ -1789,13 +1789,13 @@
         <v>30</v>
       </c>
       <c r="K30" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L30">
         <v>610.35230000000001</v>
       </c>
       <c r="M30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N30">
         <v>61.035230000000006</v>
@@ -1809,13 +1809,13 @@
         <v>33</v>
       </c>
       <c r="K31" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L31">
         <v>683.68079999999998</v>
       </c>
       <c r="M31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N31">
         <v>68.368080000000006</v>
@@ -1829,13 +1829,13 @@
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L32">
         <v>173.25665000000001</v>
       </c>
       <c r="M32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N32">
         <v>17.325665000000001</v>
@@ -1849,13 +1849,13 @@
         <v>4</v>
       </c>
       <c r="K33" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L33">
         <v>231.48813999999999</v>
       </c>
       <c r="M33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N33">
         <v>23.148814000000002</v>
@@ -1869,13 +1869,13 @@
         <v>8</v>
       </c>
       <c r="K34" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L34">
         <v>178.28899999999999</v>
       </c>
       <c r="M34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N34">
         <v>17.828900000000001</v>
@@ -1889,13 +1889,13 @@
         <v>11</v>
       </c>
       <c r="K35" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L35">
         <v>242.27173999999999</v>
       </c>
       <c r="M35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N35">
         <v>24.227174000000002</v>
@@ -1909,13 +1909,13 @@
         <v>15</v>
       </c>
       <c r="K36" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L36">
         <v>264.55786000000001</v>
       </c>
       <c r="M36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N36">
         <v>26.455786000000003</v>
@@ -1929,13 +1929,13 @@
         <v>19</v>
       </c>
       <c r="K37" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L37">
         <v>268.1524</v>
       </c>
       <c r="M37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N37">
         <v>26.815240000000003</v>
@@ -1949,13 +1949,13 @@
         <v>22</v>
       </c>
       <c r="K38" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L38">
         <v>291.87634000000003</v>
       </c>
       <c r="M38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N38">
         <v>29.187634000000003</v>
@@ -1969,13 +1969,13 @@
         <v>25</v>
       </c>
       <c r="K39" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L39">
         <v>322.07047</v>
       </c>
       <c r="M39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N39">
         <v>32.207047000000003</v>
@@ -1989,13 +1989,13 @@
         <v>30</v>
       </c>
       <c r="K40" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L40">
         <v>443.56576999999999</v>
       </c>
       <c r="M40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N40">
         <v>44.356577000000001</v>
@@ -2009,13 +2009,13 @@
         <v>33</v>
       </c>
       <c r="K41" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L41">
         <v>516.89435000000003</v>
       </c>
       <c r="M41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N41">
         <v>51.689435000000003</v>
@@ -2029,13 +2029,13 @@
         <v>1</v>
       </c>
       <c r="K42" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L42">
         <v>176.85118</v>
       </c>
       <c r="M42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N42">
         <v>17.685117999999999</v>
@@ -2049,13 +2049,13 @@
         <v>4</v>
       </c>
       <c r="K43" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L43">
         <v>226.45578</v>
       </c>
       <c r="M43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N43">
         <v>22.645578</v>
@@ -2069,13 +2069,13 @@
         <v>8</v>
       </c>
       <c r="K44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L44">
         <v>217.8289</v>
       </c>
       <c r="M44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N44">
         <v>21.782890000000002</v>
@@ -2089,13 +2089,13 @@
         <v>11</v>
       </c>
       <c r="K45" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L45">
         <v>294.75198</v>
       </c>
       <c r="M45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N45">
         <v>29.475198000000002</v>
@@ -2109,13 +2109,13 @@
         <v>15</v>
       </c>
       <c r="K46" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L46">
         <v>299.06542999999999</v>
       </c>
       <c r="M46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N46">
         <v>29.906542999999999</v>
@@ -2129,13 +2129,13 @@
         <v>19</v>
       </c>
       <c r="K47" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L47">
         <v>308.41122000000001</v>
       </c>
       <c r="M47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N47">
         <v>30.841122000000002</v>
@@ -2149,13 +2149,13 @@
         <v>22</v>
       </c>
       <c r="K48" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L48">
         <v>331.41626000000002</v>
       </c>
       <c r="M48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N48">
         <v>33.141626000000002</v>
@@ -2169,13 +2169,13 @@
         <v>25</v>
       </c>
       <c r="K49" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L49">
         <v>390.36664000000002</v>
       </c>
       <c r="M49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N49">
         <v>39.036664000000002</v>
@@ -2189,13 +2189,13 @@
         <v>30</v>
       </c>
       <c r="K50" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L50">
         <v>462.97629999999998</v>
       </c>
       <c r="M50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N50">
         <v>46.297629999999998</v>
@@ -2209,13 +2209,13 @@
         <v>33</v>
       </c>
       <c r="K51" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L51">
         <v>539.89935000000003</v>
       </c>
       <c r="M51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N51">
         <v>53.989935000000003</v>
@@ -2288,17 +2288,17 @@
       <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>6</v>
@@ -2307,16 +2307,16 @@
         <v>7</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -2327,7 +2327,7 @@
         <v>1.97137548367323</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2">
         <v>5.9562044261688006E-2</v>
@@ -2344,7 +2344,7 @@
         <v>5.2484771476368604</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3">
         <v>0.125992886970513</v>
@@ -2361,7 +2361,7 @@
         <v>9.6900340965686294</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4">
         <v>0.21059260347095399</v>
@@ -2378,7 +2378,7 @@
         <v>15.023465335155199</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5">
         <v>0.27258897671983301</v>
@@ -2395,7 +2395,7 @@
         <v>20.358907888183602</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>0.33646736562503898</v>
@@ -2412,7 +2412,7 @@
         <v>30.335314850524199</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7">
         <v>0.38581959467225097</v>
@@ -2429,7 +2429,7 @@
         <v>45.150178144993397</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8">
         <v>0.39115596306843498</v>
@@ -2446,7 +2446,7 @@
         <v>60.824160036778302</v>
       </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L9">
         <v>0.41466759038144702</v>
@@ -2463,7 +2463,7 @@
         <v>70</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L10">
         <v>0.19407067763684099</v>
@@ -2480,7 +2480,7 @@
         <v>74.866729516626663</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11">
         <v>0.15582219174951401</v>
@@ -2497,7 +2497,7 @@
         <v>79.822306022168888</v>
       </c>
       <c r="K12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L12">
         <v>6.3537976612196706E-2</v>
@@ -2514,7 +2514,7 @@
         <v>90.137127185464493</v>
       </c>
       <c r="K13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L13">
         <v>1.1751514112672801E-2</v>
@@ -2531,7 +2531,7 @@
         <v>100.0214261227288</v>
       </c>
       <c r="K14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L14">
         <v>1.1697234601759801E-2</v>
@@ -2548,7 +2548,7 @@
         <v>115.4075248543023</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L15">
         <v>3.4347503142498001E-2</v>
@@ -2565,7 +2565,7 @@
         <v>130.26068449320081</v>
       </c>
       <c r="K16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2626,17 +2626,17 @@
       <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>6</v>
@@ -2645,16 +2645,16 @@
         <v>7</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -2665,7 +2665,7 @@
         <v>30.005079736123442</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2">
         <v>0.16633663366336598</v>
@@ -2685,7 +2685,7 @@
         <v>30.971915352715747</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3">
         <v>0.308168316831683</v>
@@ -2705,7 +2705,7 @@
         <v>32.0126993403086</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4">
         <v>0.49306930693069301</v>
@@ -2725,7 +2725,7 @@
         <v>33.993773951742497</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5">
         <v>0.54282178217821708</v>
@@ -2745,7 +2745,7 @@
         <v>38.008383812274531</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>0.57549504950495001</v>
@@ -2765,7 +2765,7 @@
         <v>45.981906249648802</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7">
         <v>0.60074257425742505</v>
@@ -2826,17 +2826,17 @@
       <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>6</v>
@@ -2845,16 +2845,16 @@
         <v>7</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -2865,7 +2865,7 @@
         <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2">
         <v>0.1</v>
@@ -2882,7 +2882,7 @@
         <v>30.418764464328309</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3">
         <v>0.14722656182938781</v>
@@ -2899,7 +2899,7 @@
         <v>30.936289267226652</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4">
         <v>0.15218287009219073</v>
@@ -2916,7 +2916,7 @@
         <v>31.467416179418912</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5">
         <v>0.22059606173496588</v>
@@ -2933,7 +2933,7 @@
         <v>31.947938087839969</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>0.24476986729385974</v>
@@ -2950,7 +2950,7 @@
         <v>32.976927986178708</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7">
         <v>0.3450531339593812</v>
@@ -2967,7 +2967,7 @@
         <v>34.008432018462763</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8">
         <v>0.4078421947157902</v>
@@ -2984,7 +2984,7 @@
         <v>35.963719113219831</v>
       </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L9">
         <v>0.54204192346649882</v>
@@ -3001,7 +3001,7 @@
         <v>38.036074598866698</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L10">
         <v>0.52821851018901522</v>
@@ -3018,7 +3018,7 @@
         <v>39.947525512013044</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11">
         <v>0.51723291386976722</v>
@@ -3091,17 +3091,17 @@
       <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>6</v>
@@ -3110,16 +3110,16 @@
         <v>7</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -3127,13 +3127,13 @@
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -3147,13 +3147,13 @@
         <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3">
         <v>4.3267998695373535</v>
       </c>
       <c r="M3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N3">
         <v>1.9299999475479126</v>
@@ -3167,13 +3167,13 @@
         <v>50</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4">
         <v>20.090000152587891</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N4">
         <v>8.5299997329711914</v>
@@ -3187,13 +3187,13 @@
         <v>70</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5">
         <v>26.440000534057617</v>
       </c>
       <c r="M5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N5">
         <v>9.2299995422363281</v>
@@ -3207,13 +3207,13 @@
         <v>90</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>47.380001068115234</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N6">
         <v>10.079999923706055</v>
@@ -3227,13 +3227,13 @@
         <v>110</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7">
         <v>88.449996948242188</v>
       </c>
       <c r="M7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7">
         <v>3.0399999618530273</v>
@@ -3247,13 +3247,13 @@
         <v>130</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8">
         <v>100</v>
       </c>
       <c r="M8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N8">
         <v>0.62000000476837158</v>
@@ -3267,13 +3267,13 @@
         <v>10</v>
       </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -3287,13 +3287,13 @@
         <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L10">
         <v>20.399999618530273</v>
       </c>
       <c r="M10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N10">
         <v>9.5699996948242188</v>
@@ -3307,13 +3307,13 @@
         <v>50</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11">
         <v>29.899999618530273</v>
       </c>
       <c r="M11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N11">
         <v>7.2199997901916504</v>
@@ -3327,13 +3327,13 @@
         <v>70</v>
       </c>
       <c r="K12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L12">
         <v>49.900001525878906</v>
       </c>
       <c r="M12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N12">
         <v>7.7100000381469727</v>
@@ -3347,13 +3347,13 @@
         <v>90</v>
       </c>
       <c r="K13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L13">
         <v>80.900001525878906</v>
       </c>
       <c r="M13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N13">
         <v>7.880000114440918</v>
@@ -3367,13 +3367,13 @@
         <v>110</v>
       </c>
       <c r="K14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L14">
         <v>100</v>
       </c>
       <c r="M14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N14">
         <v>6.2899999618530273</v>
@@ -3387,13 +3387,13 @@
         <v>130</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L15">
         <v>90.099998474121094</v>
       </c>
       <c r="M15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N15">
         <v>8.5299997329711914</v>
@@ -3411,7 +3411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E64E9D-7A37-4C44-ABC1-67E774D19884}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -3455,17 +3455,17 @@
       <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>6</v>
@@ -3474,16 +3474,16 @@
         <v>7</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -3491,7 +3491,7 @@
         <v>30.913095474243164</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2">
         <v>222.21975708007813</v>
@@ -3508,7 +3508,7 @@
         <v>31.199090957641602</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3">
         <v>202.87785339355469</v>
@@ -3525,7 +3525,7 @@
         <v>31.292362213134766</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4">
         <v>170.62400817871094</v>
@@ -3542,7 +3542,7 @@
         <v>32.328723907470703</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5">
         <v>145.88314819335938</v>
@@ -3559,7 +3559,7 @@
         <v>33.317161560058594</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>121.14013671875</v>
@@ -3576,7 +3576,7 @@
         <v>35.361003875732422</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7">
         <v>110.02722930908203</v>
@@ -3593,7 +3593,7 @@
         <v>37.021049499511719</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8">
         <v>93.803573608398438</v>
@@ -3610,7 +3610,7 @@
         <v>40.057559967041016</v>
       </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L9">
         <v>110.91898345947266</v>
@@ -3627,7 +3627,7 @@
         <v>45.023651123046875</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L10">
         <v>86.356040954589844</v>
@@ -3644,7 +3644,7 @@
         <v>30.938276290893555</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11">
         <v>100.65204620361328</v>
@@ -3661,7 +3661,7 @@
         <v>31.350343704223633</v>
       </c>
       <c r="K12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L12">
         <v>85.273147583007813</v>
@@ -3678,7 +3678,7 @@
         <v>31.660545349121094</v>
       </c>
       <c r="K13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L13">
         <v>78.416740417480469</v>
@@ -3695,7 +3695,7 @@
         <v>33.103797912597656</v>
       </c>
       <c r="K14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L14">
         <v>60.973121643066406</v>
@@ -3712,7 +3712,7 @@
         <v>34.686233520507813</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L15">
         <v>51.223747253417969</v>
@@ -3729,7 +3729,7 @@
         <v>37.690589904785156</v>
       </c>
       <c r="K16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L16">
         <v>56.670791625976563</v>
@@ -3746,7 +3746,7 @@
         <v>40.324306488037109</v>
       </c>
       <c r="K17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L17">
         <v>45.896484375</v>
@@ -3763,7 +3763,7 @@
         <v>44.778003692626953</v>
       </c>
       <c r="K18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L18">
         <v>52.195217132568359</v>
@@ -3780,7 +3780,7 @@
         <v>52.317726135253906</v>
       </c>
       <c r="K19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L19">
         <v>41.073108673095703</v>
@@ -3817,8 +3817,8 @@
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -3891,6 +3891,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d2997880b21379c034af171036c714b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc8da3ca17bc816b72b8261a93c82e58" ns2:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -4054,40 +4069,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC49ADB-EC6A-4DF3-B319-3B0D82EDF8F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4104,10 +4086,28 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC49ADB-EC6A-4DF3-B319-3B0D82EDF8F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>